<commit_message>
Se agrego la columna para numero de sprint y se puso el numero de no puntuados en lugar de separarlos por coma
</commit_message>
<xml_diff>
--- a/Auditoria_Azure_Repos.xlsx
+++ b/Auditoria_Azure_Repos.xlsx
@@ -14,30 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Correo del analista</t>
-  </si>
-  <si>
-    <t>Nro de veces comprometido en historias de tipo "Habilitador"</t>
-  </si>
-  <si>
-    <t>Nro de veces comprometido en historias de tipo "User Story"</t>
-  </si>
-  <si>
-    <t>Nro de "bugs"</t>
-  </si>
-  <si>
-    <t>Nro de historias con estado "New"</t>
-  </si>
-  <si>
-    <t>Nro de historias con estado "Active"</t>
-  </si>
-  <si>
-    <t>Nro de historias con estado "Closed"</t>
-  </si>
-  <si>
-    <t>Nro de historias con estado "Impedimento"</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Nombre del analista</t>
+  </si>
+  <si>
+    <t>Habilitadores</t>
+  </si>
+  <si>
+    <t>Historias de Usuario</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Estado "New"</t>
+  </si>
+  <si>
+    <t>Estado "Active"</t>
+  </si>
+  <si>
+    <t>Estado "Closed"</t>
+  </si>
+  <si>
+    <t>Estado "Impedimento"</t>
   </si>
   <si>
     <t>Comprometido a X historias de usuario</t>
@@ -52,13 +55,19 @@
     <t>Numero de commits</t>
   </si>
   <si>
-    <t>afblando@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>jdlondon@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>aafranco@bancolombia.com.co</t>
+    <t>97</t>
+  </si>
+  <si>
+    <t>Andres Felipe Blandon Palacio</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Juan David Londono Agudelo</t>
+  </si>
+  <si>
+    <t>Alex Alberto Franco Cano</t>
   </si>
 </sst>
 </file>
@@ -438,16 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="12" width="40.7109375" customWidth="1"/>
+    <col min="1" max="13" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60" customHeight="1">
+    <row r="1" spans="1:13" ht="60" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,13 +493,16 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -513,20 +525,25 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2">
-        <v>0</v>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
       </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -549,33 +566,38 @@
       <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2">
-        <v>0</v>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="L3" s="2">
         <v>0</v>
       </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
       <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
@@ -583,13 +605,18 @@
         <v>0</v>
       </c>
       <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
         <v>5</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2">
-        <v>0</v>
+      <c r="K4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parametrización de la URL en archivos de configuración
</commit_message>
<xml_diff>
--- a/Auditoria_Azure_Repos.xlsx
+++ b/Auditoria_Azure_Repos.xlsx
@@ -1,111 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Nombre del analista</t>
-  </si>
-  <si>
-    <t>Habilitadores</t>
-  </si>
-  <si>
-    <t>Historias de Usuario</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Estado "New"</t>
-  </si>
-  <si>
-    <t>Estado "Active"</t>
-  </si>
-  <si>
-    <t>Estado "Closed"</t>
-  </si>
-  <si>
-    <t>Estado "Impedimento"</t>
-  </si>
-  <si>
-    <t>Puntos de Historia realizados</t>
-  </si>
-  <si>
-    <t>No puntuadas</t>
-  </si>
-  <si>
-    <t>Pull requests</t>
-  </si>
-  <si>
-    <t>Commits</t>
-  </si>
-  <si>
-    <t>Deuda téctina
-(Minutos)</t>
-  </si>
-  <si>
-    <t>Code Smell
-(Minutos)</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>Abel Fernando Gutierrez Arias</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Sin conexión a la VPN</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -123,7 +60,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -146,24 +83,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -451,111 +397,444 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="40.7109375" customWidth="1"/>
+    <col customWidth="1" max="15" min="1" width="40.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="60" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row customHeight="1" ht="60" r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sprint</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre del analista</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Habilitadores</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Historias de Usuario</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Estado "New"</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estado "Active"</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Estado "Closed"</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Estado "Impedimento"</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Puntos de Historia realizados</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Tareas</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Pull requests</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Commits</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Deuda téctina
+(Minutos)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Code Smell
+(Minutos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Natalia Pelaez Arboleda</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Natalia Pelaez Arboleda</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Abel Fernando Gutierrez Arias</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Andres Felipe Blandon Palacio</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O5" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Juan David Londono Agudelo</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O6" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Alex Alberto Franco Cano</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="D7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="G7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>26</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>18</v>
+      <c r="H7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>Sin conexión a la VPN</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>